<commit_message>
update statistics of failed devices
</commit_message>
<xml_diff>
--- a/01.5 - Devices_packet_numbers.xlsx
+++ b/01.5 - Devices_packet_numbers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e50b7f88a301451/Documents/GitHub/IoTDevID-CIC/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kahra\Desktop\CIC-IoTDevID\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{E62D585D-C7E0-4637-90CA-25D3A7DFCD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27E4D656-90C5-47A7-821C-A1F7F583304C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B51F0113-9E80-4E08-9090-F28E071C7E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Devices_packet_numbers" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="105">
   <si>
     <t>File</t>
   </si>
@@ -339,10 +339,16 @@
     <t>Test</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
     <t>ML</t>
+  </si>
+  <si>
+    <t>TYPE</t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -485,7 +491,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -665,6 +671,18 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -826,8 +844,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1183,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT57"/>
+  <dimension ref="A1:AR56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Z40" workbookViewId="0">
-      <selection activeCell="AG64" sqref="AG64"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1232,16 +1252,14 @@
     <col min="40" max="41" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="42" max="43" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="9" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1370,7 +1388,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>43</v>
       </c>
@@ -1503,14 +1521,8 @@
       <c r="AR2">
         <v>1123</v>
       </c>
-      <c r="AS2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1643,14 +1655,8 @@
       <c r="AR3">
         <v>1207</v>
       </c>
-      <c r="AS3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1783,14 +1789,8 @@
       <c r="AR4">
         <v>1052</v>
       </c>
-      <c r="AS4" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1923,14 +1923,8 @@
       <c r="AR5">
         <v>1055</v>
       </c>
-      <c r="AS5" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -2063,14 +2057,8 @@
       <c r="AR6">
         <v>1046</v>
       </c>
-      <c r="AS6" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -2203,14 +2191,8 @@
       <c r="AR7">
         <v>1156</v>
       </c>
-      <c r="AS7" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>50</v>
       </c>
@@ -2343,14 +2325,8 @@
       <c r="AR8">
         <v>1194</v>
       </c>
-      <c r="AS8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>51</v>
       </c>
@@ -2483,14 +2459,8 @@
       <c r="AR9">
         <v>1213</v>
       </c>
-      <c r="AS9" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -2623,14 +2593,8 @@
       <c r="AR10">
         <v>1171</v>
       </c>
-      <c r="AS10" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>53</v>
       </c>
@@ -2763,14 +2727,8 @@
       <c r="AR11">
         <v>1096</v>
       </c>
-      <c r="AS11" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>54</v>
       </c>
@@ -2903,14 +2861,8 @@
       <c r="AR12">
         <v>1341</v>
       </c>
-      <c r="AS12" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -3043,14 +2995,8 @@
       <c r="AR13">
         <v>1117</v>
       </c>
-      <c r="AS13" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -3183,14 +3129,8 @@
       <c r="AR14">
         <v>1116</v>
       </c>
-      <c r="AS14" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -3323,14 +3263,8 @@
       <c r="AR15">
         <v>1061</v>
       </c>
-      <c r="AS15" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -3463,14 +3397,8 @@
       <c r="AR16">
         <v>1034</v>
       </c>
-      <c r="AS16" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -3603,14 +3531,8 @@
       <c r="AR17">
         <v>1175</v>
       </c>
-      <c r="AS17" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -3743,14 +3665,8 @@
       <c r="AR18">
         <v>1556</v>
       </c>
-      <c r="AS18" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -3883,14 +3799,8 @@
       <c r="AR19">
         <v>1201</v>
       </c>
-      <c r="AS19" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>62</v>
       </c>
@@ -4023,14 +3933,8 @@
       <c r="AR20">
         <v>1053</v>
       </c>
-      <c r="AS20" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -4163,14 +4067,8 @@
       <c r="AR21">
         <v>1064</v>
       </c>
-      <c r="AS21" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -4303,14 +4201,8 @@
       <c r="AR22">
         <v>1204</v>
       </c>
-      <c r="AS22" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>65</v>
       </c>
@@ -4443,14 +4335,8 @@
       <c r="AR23">
         <v>1036</v>
       </c>
-      <c r="AS23" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT23">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -4583,14 +4469,8 @@
       <c r="AR24">
         <v>1104</v>
       </c>
-      <c r="AS24" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT24">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -4723,14 +4603,8 @@
       <c r="AR25">
         <v>1386</v>
       </c>
-      <c r="AS25" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT25">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>68</v>
       </c>
@@ -4863,14 +4737,8 @@
       <c r="AR26">
         <v>1432</v>
       </c>
-      <c r="AS26" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -5003,14 +4871,8 @@
       <c r="AR27">
         <v>1423</v>
       </c>
-      <c r="AS27" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -5143,14 +5005,8 @@
       <c r="AR28">
         <v>1509</v>
       </c>
-      <c r="AS28" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT28">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>72</v>
       </c>
@@ -5283,14 +5139,8 @@
       <c r="AR29">
         <v>1516</v>
       </c>
-      <c r="AS29" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT29">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -5423,14 +5273,8 @@
       <c r="AR30">
         <v>1432</v>
       </c>
-      <c r="AS30" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT30">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -5563,14 +5407,8 @@
       <c r="AR31">
         <v>1427</v>
       </c>
-      <c r="AS31" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT31">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -5703,14 +5541,8 @@
       <c r="AR32">
         <v>1426</v>
       </c>
-      <c r="AS32" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT32">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -5843,14 +5675,8 @@
       <c r="AR33">
         <v>1500</v>
       </c>
-      <c r="AS33" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT33">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>77</v>
       </c>
@@ -5983,14 +5809,8 @@
       <c r="AR34">
         <v>1505</v>
       </c>
-      <c r="AS34" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT34">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>78</v>
       </c>
@@ -6123,14 +5943,8 @@
       <c r="AR35">
         <v>1476</v>
       </c>
-      <c r="AS35" t="s">
-        <v>101</v>
-      </c>
-      <c r="AT35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -6263,14 +6077,8 @@
       <c r="AR36">
         <v>1423</v>
       </c>
-      <c r="AS36" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT36">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>80</v>
       </c>
@@ -6403,14 +6211,8 @@
       <c r="AR37">
         <v>1462</v>
       </c>
-      <c r="AS37" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT37">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>81</v>
       </c>
@@ -6543,14 +6345,8 @@
       <c r="AR38">
         <v>1433</v>
       </c>
-      <c r="AS38" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT38">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>82</v>
       </c>
@@ -6683,14 +6479,8 @@
       <c r="AR39">
         <v>1429</v>
       </c>
-      <c r="AS39" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT39">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>83</v>
       </c>
@@ -6823,14 +6613,8 @@
       <c r="AR40">
         <v>1422</v>
       </c>
-      <c r="AS40" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT40">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -6963,14 +6747,8 @@
       <c r="AR41">
         <v>1484</v>
       </c>
-      <c r="AS41" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT41">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -7103,14 +6881,8 @@
       <c r="AR42">
         <v>1424</v>
       </c>
-      <c r="AS42" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT42">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>86</v>
       </c>
@@ -7243,14 +7015,8 @@
       <c r="AR43">
         <v>1425</v>
       </c>
-      <c r="AS43" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT43">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>87</v>
       </c>
@@ -7383,14 +7149,8 @@
       <c r="AR44">
         <v>1425</v>
       </c>
-      <c r="AS44" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT44">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>88</v>
       </c>
@@ -7523,14 +7283,8 @@
       <c r="AR45">
         <v>1004</v>
       </c>
-      <c r="AS45" t="s">
-        <v>99</v>
-      </c>
-      <c r="AT45">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>89</v>
       </c>
@@ -7663,14 +7417,8 @@
       <c r="AR46">
         <v>1495</v>
       </c>
-      <c r="AS46" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT46">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>90</v>
       </c>
@@ -7803,14 +7551,8 @@
       <c r="AR47">
         <v>1443</v>
       </c>
-      <c r="AS47" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT47">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>91</v>
       </c>
@@ -7943,14 +7685,8 @@
       <c r="AR48">
         <v>1424</v>
       </c>
-      <c r="AS48" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT48">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>92</v>
       </c>
@@ -8083,14 +7819,8 @@
       <c r="AR49">
         <v>1432</v>
       </c>
-      <c r="AS49" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT49">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>93</v>
       </c>
@@ -8223,14 +7953,8 @@
       <c r="AR50">
         <v>1422</v>
       </c>
-      <c r="AS50" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT50">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>94</v>
       </c>
@@ -8363,14 +8087,8 @@
       <c r="AR51">
         <v>1436</v>
       </c>
-      <c r="AS51" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT51">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>95</v>
       </c>
@@ -8503,14 +8221,8 @@
       <c r="AR52">
         <v>1430</v>
       </c>
-      <c r="AS52" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT52">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="53" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>96</v>
       </c>
@@ -8643,14 +8355,8 @@
       <c r="AR53">
         <v>1578</v>
       </c>
-      <c r="AS53" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT53">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>97</v>
       </c>
@@ -8783,14 +8489,8 @@
       <c r="AR54">
         <v>1436</v>
       </c>
-      <c r="AS54" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT54">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>98</v>
       </c>
@@ -8923,14 +8623,8 @@
       <c r="AR55">
         <v>1561</v>
       </c>
-      <c r="AS55" t="s">
-        <v>100</v>
-      </c>
-      <c r="AT55">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:46" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:44" x14ac:dyDescent="0.3">
       <c r="E56">
         <f>SUM(E2:E55)</f>
         <v>383309</v>
@@ -9090,176 +8784,6 @@
       <c r="AR56">
         <f t="shared" si="0"/>
         <v>70995</v>
-      </c>
-      <c r="AS56">
-        <f>SUM(E56:AR56)</f>
-        <v>26211946</v>
-      </c>
-    </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.3">
-      <c r="E57">
-        <f>(E56/$AS$56)*100</f>
-        <v>1.4623446881814879</v>
-      </c>
-      <c r="F57">
-        <f>(F56/$AS$56)*100</f>
-        <v>2.9053546806482813</v>
-      </c>
-      <c r="G57">
-        <f t="shared" ref="G57:AR57" si="1">(G56/$AS$56)*100</f>
-        <v>2.8939591131463493</v>
-      </c>
-      <c r="H57">
-        <f t="shared" si="1"/>
-        <v>3.5636804684398484</v>
-      </c>
-      <c r="I57">
-        <f t="shared" si="1"/>
-        <v>3.9951020805551787</v>
-      </c>
-      <c r="J57">
-        <f t="shared" si="1"/>
-        <v>0.35972147966427215</v>
-      </c>
-      <c r="K57">
-        <f t="shared" si="1"/>
-        <v>5.1718022004165576</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="1"/>
-        <v>4.405594304215338</v>
-      </c>
-      <c r="M57">
-        <f t="shared" si="1"/>
-        <v>1.7358039727382317</v>
-      </c>
-      <c r="N57">
-        <f t="shared" si="1"/>
-        <v>6.2185272318201781</v>
-      </c>
-      <c r="O57">
-        <f t="shared" si="1"/>
-        <v>4.806968547852189E-3</v>
-      </c>
-      <c r="P57">
-        <f t="shared" si="1"/>
-        <v>0.27633202052224587</v>
-      </c>
-      <c r="Q57">
-        <f t="shared" si="1"/>
-        <v>2.0196592805433062</v>
-      </c>
-      <c r="R57">
-        <f t="shared" si="1"/>
-        <v>1.6846173878124122</v>
-      </c>
-      <c r="S57">
-        <f t="shared" si="1"/>
-        <v>4.7931847562939431</v>
-      </c>
-      <c r="T57">
-        <f t="shared" si="1"/>
-        <v>1.5832437622143738</v>
-      </c>
-      <c r="U57">
-        <f t="shared" si="1"/>
-        <v>1.6287802515692653</v>
-      </c>
-      <c r="V57">
-        <f t="shared" si="1"/>
-        <v>1.6176212174403226</v>
-      </c>
-      <c r="W57">
-        <f t="shared" si="1"/>
-        <v>1.4241674387700938</v>
-      </c>
-      <c r="X57">
-        <f t="shared" si="1"/>
-        <v>1.6178463056501033</v>
-      </c>
-      <c r="Y57">
-        <f t="shared" si="1"/>
-        <v>1.5298558908979898</v>
-      </c>
-      <c r="Z57">
-        <f t="shared" si="1"/>
-        <v>1.616430920466569</v>
-      </c>
-      <c r="AA57">
-        <f t="shared" si="1"/>
-        <v>3.331736605897174</v>
-      </c>
-      <c r="AB57">
-        <f t="shared" si="1"/>
-        <v>1.973008795302722</v>
-      </c>
-      <c r="AC57">
-        <f t="shared" si="1"/>
-        <v>5.3866622493423417</v>
-      </c>
-      <c r="AD57">
-        <f t="shared" si="1"/>
-        <v>9.2898596693278712</v>
-      </c>
-      <c r="AE57">
-        <f t="shared" si="1"/>
-        <v>0.73962078206631432</v>
-      </c>
-      <c r="AF57">
-        <f t="shared" si="1"/>
-        <v>6.057524305902354</v>
-      </c>
-      <c r="AG57">
-        <f t="shared" si="1"/>
-        <v>1.5035434606801037</v>
-      </c>
-      <c r="AH57">
-        <f t="shared" si="1"/>
-        <v>0.45675738840603441</v>
-      </c>
-      <c r="AI57">
-        <f t="shared" si="1"/>
-        <v>3.241243515456655</v>
-      </c>
-      <c r="AJ57">
-        <f t="shared" si="1"/>
-        <v>0.84048319037434305</v>
-      </c>
-      <c r="AK57">
-        <f t="shared" si="1"/>
-        <v>5.3460815156570218</v>
-      </c>
-      <c r="AL57">
-        <f t="shared" si="1"/>
-        <v>1.2444631161684827</v>
-      </c>
-      <c r="AM57">
-        <f t="shared" si="1"/>
-        <v>1.4610208643036271</v>
-      </c>
-      <c r="AN57">
-        <f t="shared" si="1"/>
-        <v>1.5765864922810384</v>
-      </c>
-      <c r="AO57">
-        <f t="shared" si="1"/>
-        <v>1.5673197251360123</v>
-      </c>
-      <c r="AP57">
-        <f t="shared" si="1"/>
-        <v>1.6058632197701002</v>
-      </c>
-      <c r="AQ57">
-        <f t="shared" si="1"/>
-        <v>1.5989388960285511</v>
-      </c>
-      <c r="AR57">
-        <f t="shared" si="1"/>
-        <v>0.27084978734505255</v>
-      </c>
-      <c r="AS57">
-        <f>(AS56/$AS$56)*100</f>
-        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -9269,781 +8793,624 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EC9E4D-F241-4A01-B5E0-DFA2FF2F1D3A}">
-  <dimension ref="F1:J54"/>
+  <dimension ref="G1:I55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A56" sqref="A56:XFD56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="6" max="6" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F1" t="s">
-        <v>43</v>
-      </c>
+    <row r="1" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G1" t="s">
+        <v>102</v>
+      </c>
+      <c r="H1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="1">
+        <v>20211102</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H1">
+    </row>
+    <row r="3" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="1">
+        <v>20211103</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="1">
+        <v>20211105</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="1">
+        <v>20211108</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" s="1">
+        <v>20211109</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" s="1">
+        <v>20211110</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" s="1">
+        <v>20211112</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="1">
+        <v>20211115</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="1">
+        <v>20211116</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="1">
+        <v>20211117</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="2">
+        <v>20211118</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G13" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="2">
+        <v>20211119</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" s="2">
+        <v>20211122</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="2">
+        <v>20211123</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H16" s="2">
+        <v>20211124</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="2">
+        <v>20211125</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G18" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="2">
+        <v>20211126</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G19" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="2">
+        <v>20211206</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H20" s="2">
+        <v>20211207</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H21" s="2">
+        <v>20211208</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H22" s="1">
+        <v>20211223</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H23" s="1">
+        <v>20211225</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="24" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="1">
+        <v>20211228</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H25" s="1">
+        <v>20220103</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G26" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H26" s="2">
         <v>20211102</v>
       </c>
-      <c r="I1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="I26" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G27" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H27" s="2">
+        <v>20211103</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" s="2">
+        <v>20211104</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H29" s="2">
+        <v>20211108</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G30" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" s="2">
+        <v>20211110</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G31" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H31" s="2">
+        <v>20211112</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H32" s="2">
+        <v>20211115</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G33" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H33" s="2">
+        <v>20211116</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G34" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H34" s="2">
+        <v>20211117</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G35" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H35" s="1">
+        <v>20211118</v>
+      </c>
+      <c r="I35" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H2">
-        <v>20211103</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="36" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G36" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H36" s="1">
+        <v>20211119</v>
+      </c>
+      <c r="I36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H3">
-        <v>20211105</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F4" t="s">
-        <v>47</v>
-      </c>
-      <c r="G4" t="s">
+    </row>
+    <row r="37" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G37" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H37" s="1">
+        <v>20211122</v>
+      </c>
+      <c r="I37" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H4">
-        <v>20211108</v>
-      </c>
-      <c r="I4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F5" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" t="s">
+    </row>
+    <row r="38" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G38" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H38" s="1">
+        <v>20211124</v>
+      </c>
+      <c r="I38" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H5">
-        <v>20211109</v>
-      </c>
-      <c r="I5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="39" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G39" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H39" s="1">
+        <v>20211125</v>
+      </c>
+      <c r="I39" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H6">
-        <v>20211110</v>
-      </c>
-      <c r="I6">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" t="s">
+    </row>
+    <row r="40" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G40" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H40" s="1">
+        <v>20211126</v>
+      </c>
+      <c r="I40" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H7">
-        <v>20211112</v>
-      </c>
-      <c r="I7">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G8" t="s">
+    </row>
+    <row r="41" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G41" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H41" s="1">
+        <v>20211129</v>
+      </c>
+      <c r="I41" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H8">
-        <v>20211115</v>
-      </c>
-      <c r="I8">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F9" t="s">
-        <v>52</v>
-      </c>
-      <c r="G9" t="s">
+    </row>
+    <row r="42" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G42" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H42" s="1">
+        <v>20211130</v>
+      </c>
+      <c r="I42" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H9">
-        <v>20211116</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F10" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" t="s">
+    </row>
+    <row r="43" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G43" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H43" s="1">
+        <v>20211201</v>
+      </c>
+      <c r="I43" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="H10">
-        <v>20211117</v>
-      </c>
-      <c r="I10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F11" t="s">
-        <v>54</v>
-      </c>
-      <c r="G11" t="s">
+    </row>
+    <row r="44" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G44" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H44" s="1">
+        <v>20211202</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G45" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H45" s="1">
+        <v>20211203</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G46" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H46" s="1">
+        <v>20211207</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="47" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G47" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H47" s="1">
+        <v>20211208</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="48" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H48" s="1">
+        <v>20211209</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="49" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G49" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H49" s="1">
+        <v>20211210</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G50" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H50" s="2">
+        <v>20211213</v>
+      </c>
+      <c r="I50" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H11">
-        <v>20211118</v>
-      </c>
-      <c r="I11">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F12" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" t="s">
+    </row>
+    <row r="51" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G51" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H51" s="2">
+        <v>20211215</v>
+      </c>
+      <c r="I51" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H12">
-        <v>20211119</v>
-      </c>
-      <c r="I12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F13" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" t="s">
+    </row>
+    <row r="52" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G52" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H52" s="2">
+        <v>20211216</v>
+      </c>
+      <c r="I52" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H13">
-        <v>20211122</v>
-      </c>
-      <c r="I13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F14" t="s">
-        <v>57</v>
-      </c>
-      <c r="G14" t="s">
+    </row>
+    <row r="53" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G53" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H53" s="2">
+        <v>20211220</v>
+      </c>
+      <c r="I53" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H14">
-        <v>20211123</v>
-      </c>
-      <c r="I14">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F15" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" t="s">
+    </row>
+    <row r="54" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G54" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H54" s="2">
+        <v>20211222</v>
+      </c>
+      <c r="I54" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H15">
-        <v>20211124</v>
-      </c>
-      <c r="I15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F16" t="s">
-        <v>59</v>
-      </c>
-      <c r="G16" t="s">
+    </row>
+    <row r="55" spans="7:9" x14ac:dyDescent="0.3">
+      <c r="G55" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H55" s="2">
+        <v>20211223</v>
+      </c>
+      <c r="I55" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H16">
-        <v>20211125</v>
-      </c>
-      <c r="I16">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F17" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" t="s">
-        <v>100</v>
-      </c>
-      <c r="H17">
-        <v>20211126</v>
-      </c>
-      <c r="I17">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="18" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F18" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" t="s">
-        <v>100</v>
-      </c>
-      <c r="H18">
-        <v>20211206</v>
-      </c>
-      <c r="I18">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F19" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" t="s">
-        <v>100</v>
-      </c>
-      <c r="H19">
-        <v>20211207</v>
-      </c>
-      <c r="I19">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F20" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" t="s">
-        <v>100</v>
-      </c>
-      <c r="H20">
-        <v>20211208</v>
-      </c>
-      <c r="I20">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F21" t="s">
-        <v>64</v>
-      </c>
-      <c r="G21" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21">
-        <v>20211223</v>
-      </c>
-      <c r="I21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F22" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" t="s">
-        <v>99</v>
-      </c>
-      <c r="H22">
-        <v>20211225</v>
-      </c>
-      <c r="I22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F23" t="s">
-        <v>66</v>
-      </c>
-      <c r="G23" t="s">
-        <v>99</v>
-      </c>
-      <c r="H23">
-        <v>20211228</v>
-      </c>
-      <c r="I23">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F24" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" t="s">
-        <v>99</v>
-      </c>
-      <c r="H24">
-        <v>20220103</v>
-      </c>
-      <c r="I24">
-        <v>6</v>
-      </c>
-      <c r="J24">
-        <f>COUNT("Test",G1:G24)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F25" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" t="s">
-        <v>100</v>
-      </c>
-      <c r="H25">
-        <v>20211102</v>
-      </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F26" t="s">
-        <v>70</v>
-      </c>
-      <c r="G26" t="s">
-        <v>100</v>
-      </c>
-      <c r="H26">
-        <v>20211103</v>
-      </c>
-      <c r="I26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F27" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" t="s">
-        <v>100</v>
-      </c>
-      <c r="H27">
-        <v>20211104</v>
-      </c>
-      <c r="I27">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F28" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" t="s">
-        <v>100</v>
-      </c>
-      <c r="H28">
-        <v>20211108</v>
-      </c>
-      <c r="I28">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F29" t="s">
-        <v>73</v>
-      </c>
-      <c r="G29" t="s">
-        <v>100</v>
-      </c>
-      <c r="H29">
-        <v>20211110</v>
-      </c>
-      <c r="I29">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F30" t="s">
-        <v>74</v>
-      </c>
-      <c r="G30" t="s">
-        <v>100</v>
-      </c>
-      <c r="H30">
-        <v>20211112</v>
-      </c>
-      <c r="I30">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F31" t="s">
-        <v>75</v>
-      </c>
-      <c r="G31" t="s">
-        <v>100</v>
-      </c>
-      <c r="H31">
-        <v>20211115</v>
-      </c>
-      <c r="I31">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="6:10" x14ac:dyDescent="0.3">
-      <c r="F32" t="s">
-        <v>76</v>
-      </c>
-      <c r="G32" t="s">
-        <v>100</v>
-      </c>
-      <c r="H32">
-        <v>20211116</v>
-      </c>
-      <c r="I32">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F33" t="s">
-        <v>77</v>
-      </c>
-      <c r="G33" t="s">
-        <v>100</v>
-      </c>
-      <c r="H33">
-        <v>20211117</v>
-      </c>
-      <c r="I33">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F34" t="s">
-        <v>78</v>
-      </c>
-      <c r="G34" t="s">
-        <v>99</v>
-      </c>
-      <c r="H34">
-        <v>20211118</v>
-      </c>
-      <c r="I34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F35" t="s">
-        <v>79</v>
-      </c>
-      <c r="G35" t="s">
-        <v>99</v>
-      </c>
-      <c r="H35">
-        <v>20211119</v>
-      </c>
-      <c r="I35">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F36" t="s">
-        <v>80</v>
-      </c>
-      <c r="G36" t="s">
-        <v>99</v>
-      </c>
-      <c r="H36">
-        <v>20211122</v>
-      </c>
-      <c r="I36">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F37" t="s">
-        <v>81</v>
-      </c>
-      <c r="G37" t="s">
-        <v>99</v>
-      </c>
-      <c r="H37">
-        <v>20211124</v>
-      </c>
-      <c r="I37">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F38" t="s">
-        <v>82</v>
-      </c>
-      <c r="G38" t="s">
-        <v>99</v>
-      </c>
-      <c r="H38">
-        <v>20211125</v>
-      </c>
-      <c r="I38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F39" t="s">
-        <v>83</v>
-      </c>
-      <c r="G39" t="s">
-        <v>99</v>
-      </c>
-      <c r="H39">
-        <v>20211126</v>
-      </c>
-      <c r="I39">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F40" t="s">
-        <v>84</v>
-      </c>
-      <c r="G40" t="s">
-        <v>99</v>
-      </c>
-      <c r="H40">
-        <v>20211129</v>
-      </c>
-      <c r="I40">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="41" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F41" t="s">
-        <v>85</v>
-      </c>
-      <c r="G41" t="s">
-        <v>99</v>
-      </c>
-      <c r="H41">
-        <v>20211130</v>
-      </c>
-      <c r="I41">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F42" t="s">
-        <v>86</v>
-      </c>
-      <c r="G42" t="s">
-        <v>99</v>
-      </c>
-      <c r="H42">
-        <v>20211201</v>
-      </c>
-      <c r="I42">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F43" t="s">
-        <v>87</v>
-      </c>
-      <c r="G43" t="s">
-        <v>99</v>
-      </c>
-      <c r="H43">
-        <v>20211202</v>
-      </c>
-      <c r="I43">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F44" t="s">
-        <v>88</v>
-      </c>
-      <c r="G44" t="s">
-        <v>99</v>
-      </c>
-      <c r="H44">
-        <v>20211203</v>
-      </c>
-      <c r="I44">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F45" t="s">
-        <v>89</v>
-      </c>
-      <c r="G45" t="s">
-        <v>99</v>
-      </c>
-      <c r="H45">
-        <v>20211207</v>
-      </c>
-      <c r="I45">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="46" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F46" t="s">
-        <v>90</v>
-      </c>
-      <c r="G46" t="s">
-        <v>99</v>
-      </c>
-      <c r="H46">
-        <v>20211208</v>
-      </c>
-      <c r="I46">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="47" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F47" t="s">
-        <v>91</v>
-      </c>
-      <c r="G47" t="s">
-        <v>99</v>
-      </c>
-      <c r="H47">
-        <v>20211209</v>
-      </c>
-      <c r="I47">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="48" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F48" t="s">
-        <v>92</v>
-      </c>
-      <c r="G48" t="s">
-        <v>99</v>
-      </c>
-      <c r="H48">
-        <v>20211210</v>
-      </c>
-      <c r="I48">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F49" t="s">
-        <v>93</v>
-      </c>
-      <c r="G49" t="s">
-        <v>100</v>
-      </c>
-      <c r="H49">
-        <v>20211213</v>
-      </c>
-      <c r="I49">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="50" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F50" t="s">
-        <v>94</v>
-      </c>
-      <c r="G50" t="s">
-        <v>100</v>
-      </c>
-      <c r="H50">
-        <v>20211215</v>
-      </c>
-      <c r="I50">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F51" t="s">
-        <v>95</v>
-      </c>
-      <c r="G51" t="s">
-        <v>100</v>
-      </c>
-      <c r="H51">
-        <v>20211216</v>
-      </c>
-      <c r="I51">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="52" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F52" t="s">
-        <v>96</v>
-      </c>
-      <c r="G52" t="s">
-        <v>100</v>
-      </c>
-      <c r="H52">
-        <v>20211220</v>
-      </c>
-      <c r="I52">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="53" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F53" t="s">
-        <v>97</v>
-      </c>
-      <c r="G53" t="s">
-        <v>100</v>
-      </c>
-      <c r="H53">
-        <v>20211222</v>
-      </c>
-      <c r="I53">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="6:9" x14ac:dyDescent="0.3">
-      <c r="F54" t="s">
-        <v>98</v>
-      </c>
-      <c r="G54" t="s">
-        <v>100</v>
-      </c>
-      <c r="H54">
-        <v>20211223</v>
-      </c>
-      <c r="I54">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="F1:J58">
-    <sortCondition ref="F1:F58"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>